<commit_message>
Shave down more time
</commit_message>
<xml_diff>
--- a/Tryouts.xlsx
+++ b/Tryouts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Code\Savage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEEE34FF-CA12-450B-AD30-29B975718B39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77DDEE9-52FD-4A0F-AF00-00D307455854}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="825" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{A20C6C29-36AB-41F9-A61B-8537634B0394}"/>
   </bookViews>
@@ -440,7 +440,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +489,7 @@
       </c>
       <c r="B5">
         <f>Lucas!G5</f>
-        <v>0</v>
+        <v>14.333333333333334</v>
       </c>
     </row>
   </sheetData>
@@ -505,7 +505,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,7 +628,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,45 +651,72 @@
       <c r="A2" t="s">
         <v>10</v>
       </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
       <c r="C2" t="s">
         <v>10</v>
       </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
       <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="e">
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2">
         <f>AVERAGE(B2,D2,F2)</f>
-        <v>#DIV/0!</v>
+        <v>4.666666666666667</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
       <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" t="e">
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
         <f t="shared" ref="G3:G4" si="0">AVERAGE(B3,D3,F3)</f>
-        <v>#DIV/0!</v>
+        <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
       <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="G4" t="e">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>3.3333333333333335</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -698,19 +725,19 @@
       </c>
       <c r="B5">
         <f>2*B2+B3+B4</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D5">
         <f>2*D2+D3+D4</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F5">
         <f>2*F2+F3+F4</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G5">
         <f>AVERAGE(B5,D5,F5)</f>
-        <v>0</v>
+        <v>14.333333333333334</v>
       </c>
     </row>
   </sheetData>
@@ -723,7 +750,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,7 +872,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>